<commit_message>
The second commit with Delete data and save customer ID
</commit_message>
<xml_diff>
--- a/src/test/java/org/example/testData/Login_Data.xlsx
+++ b/src/test/java/org/example/testData/Login_Data.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Customer" sheetId="2" r:id="rId2"/>
+    <sheet name="CusID" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t>Username</t>
   </si>
@@ -118,7 +119,22 @@
     <t>555 McDermott Path Suite 018</t>
   </si>
   <si>
-    <t>rdate.rei654657@gmail.com</t>
+    <t xml:space="preserve">Customer Name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email Id </t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Customer ID</t>
+  </si>
+  <si>
+    <t>rdete.rei654657@gmail.com</t>
+  </si>
+  <si>
+    <t>rdesfgate657@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -649,7 +665,7 @@
         <v>8174470105</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="J2" t="s">
         <v>29</v>
@@ -662,4 +678,50 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView zoomScale="129" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2">
+        <v>8174470105</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>